<commit_message>
Tested all sample and fix 1 bug
</commit_message>
<xml_diff>
--- a/TA/Plagiarism Checker/Rumus baru fix.xlsx
+++ b/TA/Plagiarism Checker/Rumus baru fix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wisely\Downloads\Plagiarism Checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="9">
   <si>
     <t>leven</t>
   </si>
@@ -46,11 +46,17 @@
   <si>
     <t>Preprocessing</t>
   </si>
+  <si>
+    <t>Benar</t>
+  </si>
+  <si>
+    <t>Benaar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:P81"/>
+  <dimension ref="D1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>5</v>
       </c>
@@ -385,7 +391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>0</v>
       </c>
@@ -403,7 +409,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>1</v>
       </c>
@@ -421,7 +427,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G5" s="1"/>
       <c r="H5" s="1">
         <f>(G3/G9/2)*100</f>
@@ -441,7 +447,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>1</v>
       </c>
@@ -461,7 +467,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>2</v>
       </c>
@@ -470,6 +476,9 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
       <c r="M7" t="s">
         <v>2</v>
       </c>
@@ -479,7 +488,10 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
       <c r="F8" t="s">
         <v>3</v>
       </c>
@@ -497,7 +509,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>4</v>
       </c>
@@ -517,7 +529,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>0</v>
       </c>
@@ -535,7 +547,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>1</v>
       </c>
@@ -553,7 +565,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
       <c r="H13" s="1">
         <f>(G11/G17/2)*100</f>
@@ -573,7 +585,10 @@
         <v>31.014492753623188</v>
       </c>
     </row>
-    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
       <c r="E14">
         <v>2</v>
       </c>
@@ -583,6 +598,9 @@
         <v>16.521739130434781</v>
       </c>
       <c r="I14" s="1"/>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
       <c r="L14">
         <v>2</v>
       </c>
@@ -593,7 +611,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>2</v>
       </c>
@@ -611,7 +629,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>3</v>
       </c>
@@ -629,7 +647,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>4</v>
       </c>
@@ -649,7 +667,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>0</v>
       </c>
@@ -667,7 +685,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>1</v>
       </c>
@@ -685,7 +703,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
       <c r="H21" s="1">
         <f>(G19/G25/2)*100</f>
@@ -705,7 +723,10 @@
         <v>20.673076923076923</v>
       </c>
     </row>
-    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
       <c r="E22">
         <v>3</v>
       </c>
@@ -715,6 +736,9 @@
         <v>16.826923076923077</v>
       </c>
       <c r="I22" s="1"/>
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
       <c r="L22">
         <v>3</v>
       </c>
@@ -725,7 +749,7 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>2</v>
       </c>
@@ -743,7 +767,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>3</v>
       </c>
@@ -761,7 +785,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>4</v>
       </c>
@@ -781,7 +805,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>0</v>
       </c>
@@ -799,7 +823,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>1</v>
       </c>
@@ -817,7 +841,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G29" s="1"/>
       <c r="H29" s="1">
         <f>(G27/G33/2)*100</f>
@@ -837,7 +861,10 @@
         <v>24.686192468619247</v>
       </c>
     </row>
-    <row r="30" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
       <c r="E30">
         <v>4</v>
       </c>
@@ -847,6 +874,9 @@
         <v>30.753138075313807</v>
       </c>
       <c r="I30" s="1"/>
+      <c r="K30" t="s">
+        <v>7</v>
+      </c>
       <c r="L30">
         <v>4</v>
       </c>
@@ -857,7 +887,7 @@
       </c>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>2</v>
       </c>
@@ -875,7 +905,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>3</v>
       </c>
@@ -893,7 +923,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>4</v>
       </c>
@@ -913,7 +943,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>0</v>
       </c>
@@ -931,7 +961,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>1</v>
       </c>
@@ -949,7 +979,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G37" s="1"/>
       <c r="H37" s="1">
         <f>(G35/G41/2)*100</f>
@@ -969,7 +999,10 @@
         <v>18.814432989690722</v>
       </c>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
       <c r="E38">
         <v>5</v>
       </c>
@@ -979,6 +1012,9 @@
         <v>14.690721649484537</v>
       </c>
       <c r="I38" s="1"/>
+      <c r="K38" t="s">
+        <v>7</v>
+      </c>
       <c r="L38">
         <v>5</v>
       </c>
@@ -989,7 +1025,7 @@
       </c>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1043,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1061,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>4</v>
       </c>
@@ -1045,7 +1081,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1099,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>1</v>
       </c>
@@ -1081,7 +1117,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G45" s="1"/>
       <c r="H45" s="1">
         <f>(G43/G49/2)*100</f>
@@ -1101,7 +1137,10 @@
         <v>49.609375</v>
       </c>
     </row>
-    <row r="46" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
       <c r="E46">
         <v>6</v>
       </c>
@@ -1111,6 +1150,9 @@
         <v>29.58984375</v>
       </c>
       <c r="I46" s="1"/>
+      <c r="K46" t="s">
+        <v>7</v>
+      </c>
       <c r="L46">
         <v>6</v>
       </c>
@@ -1121,7 +1163,7 @@
       </c>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>2</v>
       </c>
@@ -1139,7 +1181,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>3</v>
       </c>
@@ -1157,7 +1199,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>4</v>
       </c>
@@ -1177,7 +1219,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="51" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1237,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
         <v>1</v>
       </c>
@@ -1213,7 +1255,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G53" s="1"/>
       <c r="H53" s="1">
         <f>(G51/G57/2)*100</f>
@@ -1233,7 +1275,10 @@
         <v>20.087336244541486</v>
       </c>
     </row>
-    <row r="54" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
       <c r="E54">
         <v>7</v>
       </c>
@@ -1243,6 +1288,9 @@
         <v>14.192139737991265</v>
       </c>
       <c r="I54" s="1"/>
+      <c r="K54" t="s">
+        <v>7</v>
+      </c>
       <c r="L54">
         <v>7</v>
       </c>
@@ -1253,7 +1301,7 @@
       </c>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
         <v>2</v>
       </c>
@@ -1271,7 +1319,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
         <v>3</v>
       </c>
@@ -1289,7 +1337,7 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
         <v>4</v>
       </c>
@@ -1309,7 +1357,7 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="59" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1375,7 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
         <v>1</v>
       </c>
@@ -1345,7 +1393,7 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G61" s="1"/>
       <c r="H61" s="1">
         <f>(G59/G65/2)*100</f>
@@ -1365,7 +1413,10 @@
         <v>37.47152619589977</v>
       </c>
     </row>
-    <row r="62" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
       <c r="E62">
         <v>8</v>
       </c>
@@ -1375,6 +1426,9 @@
         <v>24.829157175398635</v>
       </c>
       <c r="I62" s="1"/>
+      <c r="K62" t="s">
+        <v>7</v>
+      </c>
       <c r="L62">
         <v>8</v>
       </c>
@@ -1385,7 +1439,7 @@
       </c>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
         <v>2</v>
       </c>
@@ -1403,7 +1457,7 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>3</v>
       </c>
@@ -1421,7 +1475,7 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1495,7 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="67" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1513,7 @@
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1531,10 @@
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
       <c r="E69">
         <v>9</v>
       </c>
@@ -1490,6 +1547,9 @@
         <f>(H69+H70)</f>
         <v>52.10280373831776</v>
       </c>
+      <c r="K69" t="s">
+        <v>7</v>
+      </c>
       <c r="L69">
         <v>9</v>
       </c>
@@ -1503,7 +1563,7 @@
         <v>40.887850467289717</v>
       </c>
     </row>
-    <row r="70" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G70" s="1"/>
       <c r="H70" s="1">
         <f>(G68/G73/2)*100</f>
@@ -1517,7 +1577,7 @@
       </c>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
         <v>2</v>
       </c>
@@ -1535,7 +1595,7 @@
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
         <v>3</v>
       </c>
@@ -1553,7 +1613,7 @@
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>4</v>
       </c>
@@ -1573,7 +1633,7 @@
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="75" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1651,7 @@
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>1</v>
       </c>
@@ -1609,7 +1669,10 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
       <c r="E77">
         <v>10</v>
       </c>
@@ -1622,6 +1685,9 @@
         <f>(H77+H78)</f>
         <v>52.709359605911331</v>
       </c>
+      <c r="K77" t="s">
+        <v>7</v>
+      </c>
       <c r="L77">
         <v>10</v>
       </c>
@@ -1635,7 +1701,7 @@
         <v>38.669950738916256</v>
       </c>
     </row>
-    <row r="78" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:16" x14ac:dyDescent="0.25">
       <c r="G78" s="1"/>
       <c r="H78" s="1">
         <f>(G76/G81/2)*100</f>
@@ -1649,7 +1715,7 @@
       </c>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
         <v>2</v>
       </c>
@@ -1667,7 +1733,7 @@
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
     </row>
-    <row r="80" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:16" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
         <v>3</v>
       </c>

</xml_diff>